<commit_message>
integrated service and set values in game
</commit_message>
<xml_diff>
--- a/GamePlanMemory.xlsx
+++ b/GamePlanMemory.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8AF230-2B5E-4401-98D2-3058E3726812}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D5B8C6-B6FD-4E98-ADDE-15906D641378}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -355,12 +355,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,12 +368,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>

</xml_diff>